<commit_message>
This is the 0th saving data.
</commit_message>
<xml_diff>
--- a/Stocks/AAPL/AAPL_HighLow.xlsx
+++ b/Stocks/AAPL/AAPL_HighLow.xlsx
@@ -417,2562 +417,2562 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>129.8000030517578</v>
+        <v>133.5099945068359</v>
       </c>
       <c r="B2">
-        <v>133.0399932861328</v>
+        <v>135.4700012207031</v>
       </c>
       <c r="C2">
-        <v>129.4700012207031</v>
+        <v>133.3399963378906</v>
       </c>
       <c r="D2">
-        <v>133</v>
+        <v>134.8399963378906</v>
       </c>
       <c r="E2">
-        <v>132.5758361816406</v>
+        <v>134.4099578857422</v>
       </c>
       <c r="F2">
-        <v>106686700</v>
+        <v>94264200</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>132.5200042724609</v>
+        <v>135.0200042724609</v>
       </c>
       <c r="B3">
-        <v>132.8500061035156</v>
+        <v>135.5299987792969</v>
       </c>
       <c r="C3">
-        <v>130.6300048828125</v>
+        <v>131.8099975585938</v>
       </c>
       <c r="D3">
-        <v>131.2400054931641</v>
+        <v>133.1100006103516</v>
       </c>
       <c r="E3">
-        <v>130.8214569091797</v>
+        <v>132.6855010986328</v>
       </c>
       <c r="F3">
-        <v>91420000</v>
+        <v>94812300</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>132.4400024414062</v>
+        <v>132.3600006103516</v>
       </c>
       <c r="B4">
-        <v>134.6600036621094</v>
+        <v>133.75</v>
       </c>
       <c r="C4">
-        <v>131.9299926757812</v>
+        <v>131.3000030517578</v>
       </c>
       <c r="D4">
-        <v>134.4299926757812</v>
+        <v>133.5</v>
       </c>
       <c r="E4">
-        <v>134.0012664794922</v>
+        <v>133.0742340087891</v>
       </c>
       <c r="F4">
-        <v>91266500</v>
+        <v>68847100</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>134.9400024414062</v>
+        <v>133.0399932861328</v>
       </c>
       <c r="B5">
-        <v>135</v>
+        <v>134.1499938964844</v>
       </c>
       <c r="C5">
-        <v>131.6600036621094</v>
+        <v>131.4100036621094</v>
       </c>
       <c r="D5">
-        <v>132.0299987792969</v>
+        <v>131.9400024414062</v>
       </c>
       <c r="E5">
-        <v>131.6089324951172</v>
+        <v>131.5192260742188</v>
       </c>
       <c r="F5">
-        <v>87222800</v>
+        <v>84566500</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>133.8200073242188</v>
+        <v>132.1600036621094</v>
       </c>
       <c r="B6">
-        <v>135</v>
+        <v>135.1199951171875</v>
       </c>
       <c r="C6">
-        <v>133.6399993896484</v>
+        <v>132.1600036621094</v>
       </c>
       <c r="D6">
-        <v>134.5</v>
+        <v>134.3200073242188</v>
       </c>
       <c r="E6">
-        <v>134.0710601806641</v>
+        <v>133.8916320800781</v>
       </c>
       <c r="F6">
-        <v>89347100</v>
+        <v>78657500</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>134.3000030517578</v>
+        <v>134.8300018310547</v>
       </c>
       <c r="B7">
-        <v>134.6699981689453</v>
+        <v>135.0599975585938</v>
       </c>
       <c r="C7">
-        <v>133.2799987792969</v>
+        <v>133.5599975585938</v>
       </c>
       <c r="D7">
-        <v>134.1600036621094</v>
+        <v>134.7200012207031</v>
       </c>
       <c r="E7">
-        <v>133.7321472167969</v>
+        <v>134.2903594970703</v>
       </c>
       <c r="F7">
-        <v>84922400</v>
+        <v>66905100</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>133.5099945068359</v>
+        <v>135.0099945068359</v>
       </c>
       <c r="B8">
-        <v>135.4700012207031</v>
+        <v>135.4100036621094</v>
       </c>
       <c r="C8">
-        <v>133.3399963378906</v>
+        <v>134.1100006103516</v>
       </c>
       <c r="D8">
-        <v>134.8399963378906</v>
+        <v>134.3899993896484</v>
       </c>
       <c r="E8">
-        <v>134.4099731445312</v>
+        <v>133.9613952636719</v>
       </c>
       <c r="F8">
-        <v>94264200</v>
+        <v>66015800</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
+        <v>134.3099975585938</v>
+      </c>
+      <c r="B9">
         <v>135.0200042724609</v>
       </c>
-      <c r="B9">
-        <v>135.5299987792969</v>
-      </c>
       <c r="C9">
-        <v>131.8099975585938</v>
+        <v>133.0800018310547</v>
       </c>
       <c r="D9">
-        <v>133.1100006103516</v>
+        <v>133.5800018310547</v>
       </c>
       <c r="E9">
-        <v>132.6855010986328</v>
+        <v>133.1539916992188</v>
       </c>
       <c r="F9">
-        <v>94812300</v>
+        <v>107760100</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>132.3600006103516</v>
+        <v>136.4700012207031</v>
       </c>
       <c r="B10">
-        <v>133.75</v>
+        <v>137.0700073242188</v>
       </c>
       <c r="C10">
-        <v>131.3000030517578</v>
+        <v>132.4499969482422</v>
       </c>
       <c r="D10">
-        <v>133.5</v>
+        <v>133.4799957275391</v>
       </c>
       <c r="E10">
-        <v>133.0742340087891</v>
+        <v>133.0543060302734</v>
       </c>
       <c r="F10">
-        <v>68847100</v>
+        <v>151101000</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>133.0399932861328</v>
+        <v>131.7799987792969</v>
       </c>
       <c r="B11">
-        <v>134.1499938964844</v>
+        <v>133.5599975585938</v>
       </c>
       <c r="C11">
-        <v>131.4100036621094</v>
+        <v>131.0700073242188</v>
       </c>
       <c r="D11">
-        <v>131.9400024414062</v>
+        <v>131.4600067138672</v>
       </c>
       <c r="E11">
-        <v>131.5192260742188</v>
+        <v>131.0407562255859</v>
       </c>
       <c r="F11">
-        <v>84566500</v>
+        <v>109839500</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>132.1600036621094</v>
+        <v>132.0399932861328</v>
       </c>
       <c r="B12">
-        <v>135.1199951171875</v>
+        <v>134.0700073242188</v>
       </c>
       <c r="C12">
-        <v>132.1600036621094</v>
+        <v>131.8300018310547</v>
       </c>
       <c r="D12">
-        <v>134.3200073242188</v>
+        <v>132.5399932861328</v>
       </c>
       <c r="E12">
-        <v>133.8916320800781</v>
+        <v>132.1172943115234</v>
       </c>
       <c r="F12">
-        <v>78657500</v>
+        <v>75135100</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>134.8300018310547</v>
+        <v>131.1900024414062</v>
       </c>
       <c r="B13">
-        <v>135.0599975585938</v>
+        <v>131.4900054931641</v>
       </c>
       <c r="C13">
-        <v>133.5599975585938</v>
+        <v>126.6999969482422</v>
       </c>
       <c r="D13">
-        <v>134.7200012207031</v>
+        <v>127.8499984741211</v>
       </c>
       <c r="E13">
-        <v>134.2903594970703</v>
+        <v>127.4422607421875</v>
       </c>
       <c r="F13">
-        <v>66905100</v>
+        <v>137564700</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>135.0099945068359</v>
+        <v>129.1999969482422</v>
       </c>
       <c r="B14">
-        <v>135.4100036621094</v>
+        <v>130.4499969482422</v>
       </c>
       <c r="C14">
-        <v>134.1100006103516</v>
+        <v>127.9700012207031</v>
       </c>
       <c r="D14">
-        <v>134.3899993896484</v>
+        <v>128.1000061035156</v>
       </c>
       <c r="E14">
-        <v>133.9614105224609</v>
+        <v>127.6914749145508</v>
       </c>
       <c r="F14">
-        <v>66015800</v>
+        <v>84000900</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>134.3099975585938</v>
+        <v>127.8899993896484</v>
       </c>
       <c r="B15">
-        <v>135.0200042724609</v>
+        <v>129.75</v>
       </c>
       <c r="C15">
-        <v>133.0800018310547</v>
+        <v>127.129997253418</v>
       </c>
       <c r="D15">
-        <v>133.5800018310547</v>
+        <v>129.7400054931641</v>
       </c>
       <c r="E15">
-        <v>133.1539916992188</v>
+        <v>129.3262329101562</v>
       </c>
       <c r="F15">
-        <v>107760100</v>
+        <v>78128300</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>136.4700012207031</v>
+        <v>130.8500061035156</v>
       </c>
       <c r="B16">
-        <v>137.0700073242188</v>
+        <v>131.2599945068359</v>
       </c>
       <c r="C16">
-        <v>132.4499969482422</v>
+        <v>129.4799957275391</v>
       </c>
       <c r="D16">
-        <v>133.4799957275391</v>
+        <v>130.2100067138672</v>
       </c>
       <c r="E16">
-        <v>133.0543060302734</v>
+        <v>130.0152130126953</v>
       </c>
       <c r="F16">
-        <v>151101000</v>
+        <v>78973300</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>131.7799987792969</v>
+        <v>129.4100036621094</v>
       </c>
       <c r="B17">
-        <v>133.5599975585938</v>
+        <v>129.5399932861328</v>
       </c>
       <c r="C17">
-        <v>131.0700073242188</v>
+        <v>126.8099975585938</v>
       </c>
       <c r="D17">
-        <v>131.4600067138672</v>
+        <v>126.8499984741211</v>
       </c>
       <c r="E17">
-        <v>131.0407562255859</v>
+        <v>126.6602249145508</v>
       </c>
       <c r="F17">
-        <v>109839500</v>
+        <v>88071200</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>132.0399932861328</v>
+        <v>123.5</v>
       </c>
       <c r="B18">
-        <v>134.0700073242188</v>
+        <v>126.2699966430664</v>
       </c>
       <c r="C18">
-        <v>131.8300018310547</v>
+        <v>122.7699966430664</v>
       </c>
       <c r="D18">
-        <v>132.5399932861328</v>
+        <v>125.9100036621094</v>
       </c>
       <c r="E18">
-        <v>132.1172943115234</v>
+        <v>125.7216415405273</v>
       </c>
       <c r="F18">
-        <v>75135100</v>
+        <v>126142800</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>131.1900024414062</v>
+        <v>123.4000015258789</v>
       </c>
       <c r="B19">
-        <v>131.4900054931641</v>
+        <v>124.6399993896484</v>
       </c>
       <c r="C19">
-        <v>126.6999969482422</v>
+        <v>122.25</v>
       </c>
       <c r="D19">
-        <v>127.8499984741211</v>
+        <v>122.7699966430664</v>
       </c>
       <c r="E19">
-        <v>127.4422607421875</v>
+        <v>122.5863342285156</v>
       </c>
       <c r="F19">
-        <v>137564700</v>
+        <v>112172300</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>129.1999969482422</v>
+        <v>124.5800018310547</v>
       </c>
       <c r="B20">
-        <v>130.4499969482422</v>
+        <v>126.1500015258789</v>
       </c>
       <c r="C20">
-        <v>127.9700012207031</v>
+        <v>124.2600021362305</v>
       </c>
       <c r="D20">
-        <v>128.1000061035156</v>
+        <v>124.9700012207031</v>
       </c>
       <c r="E20">
-        <v>127.6914672851562</v>
+        <v>124.7830429077148</v>
       </c>
       <c r="F20">
-        <v>84000900</v>
+        <v>105861300</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
+        <v>126.25</v>
+      </c>
+      <c r="B21">
         <v>127.8899993896484</v>
       </c>
-      <c r="B21">
-        <v>129.75</v>
-      </c>
       <c r="C21">
-        <v>127.129997253418</v>
+        <v>125.8499984741211</v>
       </c>
       <c r="D21">
-        <v>129.7400054931641</v>
+        <v>127.4499969482422</v>
       </c>
       <c r="E21">
-        <v>129.3262481689453</v>
+        <v>127.2593307495117</v>
       </c>
       <c r="F21">
-        <v>78128300</v>
+        <v>81918000</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>130.8500061035156</v>
+        <v>126.8199996948242</v>
       </c>
       <c r="B22">
-        <v>131.2599945068359</v>
+        <v>126.9300003051758</v>
       </c>
       <c r="C22">
-        <v>129.4799957275391</v>
+        <v>125.1699981689453</v>
       </c>
       <c r="D22">
-        <v>130.2100067138672</v>
+        <v>126.2699966430664</v>
       </c>
       <c r="E22">
-        <v>130.0152130126953</v>
+        <v>126.0810928344727</v>
       </c>
       <c r="F22">
-        <v>78973300</v>
+        <v>74244600</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>129.4100036621094</v>
+        <v>126.5599975585938</v>
       </c>
       <c r="B23">
-        <v>129.5399932861328</v>
+        <v>126.9899978637695</v>
       </c>
       <c r="C23">
-        <v>126.8099975585938</v>
+        <v>124.7799987792969</v>
       </c>
       <c r="D23">
-        <v>126.8499984741211</v>
+        <v>124.8499984741211</v>
       </c>
       <c r="E23">
-        <v>126.6602249145508</v>
+        <v>124.6632232666016</v>
       </c>
       <c r="F23">
-        <v>88071200</v>
+        <v>63342900</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>123.5</v>
+        <v>123.1600036621094</v>
       </c>
       <c r="B24">
-        <v>126.2699966430664</v>
+        <v>124.9199981689453</v>
       </c>
       <c r="C24">
-        <v>122.7699966430664</v>
+        <v>122.8600006103516</v>
       </c>
       <c r="D24">
-        <v>125.9100036621094</v>
+        <v>124.6900024414062</v>
       </c>
       <c r="E24">
-        <v>125.7216415405273</v>
+        <v>124.5034637451172</v>
       </c>
       <c r="F24">
-        <v>126142800</v>
+        <v>92612000</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>123.4000015258789</v>
+        <v>125.2300033569336</v>
       </c>
       <c r="B25">
-        <v>124.6399993896484</v>
+        <v>127.7200012207031</v>
       </c>
       <c r="C25">
-        <v>122.25</v>
+        <v>125.0999984741211</v>
       </c>
       <c r="D25">
-        <v>122.7699966430664</v>
+        <v>127.3099975585938</v>
       </c>
       <c r="E25">
-        <v>122.5863342285156</v>
+        <v>127.1195373535156</v>
       </c>
       <c r="F25">
-        <v>112172300</v>
+        <v>76857100</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>124.5800018310547</v>
+        <v>127.8199996948242</v>
       </c>
       <c r="B26">
-        <v>126.1500015258789</v>
+        <v>128</v>
       </c>
       <c r="C26">
-        <v>124.2600021362305</v>
+        <v>125.2099990844727</v>
       </c>
       <c r="D26">
-        <v>124.9700012207031</v>
+        <v>125.4300003051758</v>
       </c>
       <c r="E26">
-        <v>124.7830429077148</v>
+        <v>125.2423553466797</v>
       </c>
       <c r="F26">
-        <v>105861300</v>
+        <v>79295400</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27">
-        <v>126.25</v>
+        <v>126.0100021362305</v>
       </c>
       <c r="B27">
-        <v>127.8899993896484</v>
+        <v>127.9400024414062</v>
       </c>
       <c r="C27">
-        <v>125.8499984741211</v>
+        <v>125.9400024414062</v>
       </c>
       <c r="D27">
-        <v>127.4499969482422</v>
+        <v>127.0999984741211</v>
       </c>
       <c r="E27">
-        <v>127.2593307495117</v>
+        <v>126.9098510742188</v>
       </c>
       <c r="F27">
-        <v>81918000</v>
+        <v>63092900</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>126.8199996948242</v>
+        <v>127.8199996948242</v>
       </c>
       <c r="B28">
-        <v>126.9300003051758</v>
+        <v>128.3200073242188</v>
       </c>
       <c r="C28">
-        <v>125.1699981689453</v>
+        <v>126.3199996948242</v>
       </c>
       <c r="D28">
-        <v>126.2699966430664</v>
+        <v>126.9000015258789</v>
       </c>
       <c r="E28">
-        <v>126.0810928344727</v>
+        <v>126.7101593017578</v>
       </c>
       <c r="F28">
-        <v>74244600</v>
+        <v>72009500</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>126.5599975585938</v>
+        <v>126.9599990844727</v>
       </c>
       <c r="B29">
-        <v>126.9899978637695</v>
+        <v>127.3899993896484</v>
       </c>
       <c r="C29">
-        <v>124.7799987792969</v>
+        <v>126.4199981689453</v>
       </c>
       <c r="D29">
-        <v>124.8499984741211</v>
+        <v>126.8499984741211</v>
       </c>
       <c r="E29">
-        <v>124.6632232666016</v>
+        <v>126.6602249145508</v>
       </c>
       <c r="F29">
-        <v>63342900</v>
+        <v>56575900</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>123.1600036621094</v>
+        <v>126.4400024414062</v>
       </c>
       <c r="B30">
-        <v>124.9199981689453</v>
+        <v>127.6399993896484</v>
       </c>
       <c r="C30">
-        <v>122.8600006103516</v>
+        <v>125.0800018310547</v>
       </c>
       <c r="D30">
-        <v>124.6900024414062</v>
+        <v>125.2799987792969</v>
       </c>
       <c r="E30">
-        <v>124.5034637451172</v>
+        <v>125.0925750732422</v>
       </c>
       <c r="F30">
-        <v>92612000</v>
+        <v>94625600</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
-        <v>125.2300033569336</v>
+        <v>125.5699996948242</v>
       </c>
       <c r="B31">
-        <v>127.7200012207031</v>
+        <v>125.8000030517578</v>
       </c>
       <c r="C31">
-        <v>125.0999984741211</v>
+        <v>124.5500030517578</v>
       </c>
       <c r="D31">
-        <v>127.3099975585938</v>
+        <v>124.6100006103516</v>
       </c>
       <c r="E31">
-        <v>127.1195373535156</v>
+        <v>124.423583984375</v>
       </c>
       <c r="F31">
-        <v>76857100</v>
+        <v>71311100</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>127.8199996948242</v>
+        <v>125.0800018310547</v>
       </c>
       <c r="B32">
-        <v>128</v>
+        <v>125.3499984741211</v>
       </c>
       <c r="C32">
-        <v>125.2099990844727</v>
+        <v>123.9400024414062</v>
       </c>
       <c r="D32">
-        <v>125.4300003051758</v>
+        <v>124.2799987792969</v>
       </c>
       <c r="E32">
-        <v>125.2423553466797</v>
+        <v>124.0940704345703</v>
       </c>
       <c r="F32">
-        <v>79295400</v>
+        <v>67637100</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>126.0100021362305</v>
+        <v>124.2799987792969</v>
       </c>
       <c r="B33">
-        <v>127.9400024414062</v>
+        <v>125.2399978637695</v>
       </c>
       <c r="C33">
-        <v>125.9400024414062</v>
+        <v>124.0500030517578</v>
       </c>
       <c r="D33">
-        <v>127.0999984741211</v>
+        <v>125.0599975585938</v>
       </c>
       <c r="E33">
-        <v>126.9098510742188</v>
+        <v>124.8729019165039</v>
       </c>
       <c r="F33">
-        <v>63092900</v>
+        <v>59278900</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>127.8199996948242</v>
+        <v>124.6800003051758</v>
       </c>
       <c r="B34">
-        <v>128.3200073242188</v>
+        <v>124.8499984741211</v>
       </c>
       <c r="C34">
-        <v>126.3199996948242</v>
+        <v>123.129997253418</v>
       </c>
       <c r="D34">
-        <v>126.9000015258789</v>
+        <v>123.5400009155273</v>
       </c>
       <c r="E34">
-        <v>126.7101593017578</v>
+        <v>123.3551864624023</v>
       </c>
       <c r="F34">
-        <v>72009500</v>
+        <v>76229200</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>126.9599990844727</v>
+        <v>124.0699996948242</v>
       </c>
       <c r="B35">
-        <v>127.3899993896484</v>
+        <v>126.1600036621094</v>
       </c>
       <c r="C35">
-        <v>126.4199981689453</v>
+        <v>123.8499984741211</v>
       </c>
       <c r="D35">
-        <v>126.8499984741211</v>
+        <v>125.8899993896484</v>
       </c>
       <c r="E35">
-        <v>126.6602249145508</v>
+        <v>125.7016677856445</v>
       </c>
       <c r="F35">
-        <v>56575900</v>
+        <v>75169300</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>126.4400024414062</v>
+        <v>126.1699981689453</v>
       </c>
       <c r="B36">
-        <v>127.6399993896484</v>
+        <v>126.3199996948242</v>
       </c>
       <c r="C36">
-        <v>125.0800018310547</v>
+        <v>124.8300018310547</v>
       </c>
       <c r="D36">
-        <v>125.2799987792969</v>
+        <v>125.9000015258789</v>
       </c>
       <c r="E36">
-        <v>125.0925750732422</v>
+        <v>125.7116546630859</v>
       </c>
       <c r="F36">
-        <v>94625600</v>
+        <v>71057600</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>125.5699996948242</v>
+        <v>126.5999984741211</v>
       </c>
       <c r="B37">
-        <v>125.8000030517578</v>
+        <v>128.4600067138672</v>
       </c>
       <c r="C37">
-        <v>124.5500030517578</v>
+        <v>126.2099990844727</v>
       </c>
       <c r="D37">
-        <v>124.6100006103516</v>
+        <v>126.7399978637695</v>
       </c>
       <c r="E37">
-        <v>124.423583984375</v>
+        <v>126.5503921508789</v>
       </c>
       <c r="F37">
-        <v>71311100</v>
+        <v>74403800</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>125.0800018310547</v>
+        <v>127.2099990844727</v>
       </c>
       <c r="B38">
-        <v>125.3499984741211</v>
+        <v>127.75</v>
       </c>
       <c r="C38">
-        <v>123.9400024414062</v>
+        <v>126.5199966430664</v>
       </c>
       <c r="D38">
-        <v>124.2799987792969</v>
+        <v>127.129997253418</v>
       </c>
       <c r="E38">
-        <v>124.0940704345703</v>
+        <v>126.939811706543</v>
       </c>
       <c r="F38">
-        <v>67637100</v>
+        <v>56877900</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
-        <v>124.2799987792969</v>
+        <v>127.0199966430664</v>
       </c>
       <c r="B39">
-        <v>125.2399978637695</v>
+        <v>128.1900024414062</v>
       </c>
       <c r="C39">
-        <v>124.0500030517578</v>
+        <v>125.9400024414062</v>
       </c>
       <c r="D39">
-        <v>125.0599975585938</v>
+        <v>126.1100006103516</v>
       </c>
       <c r="E39">
-        <v>124.8729019165039</v>
+        <v>125.9213409423828</v>
       </c>
       <c r="F39">
-        <v>59278900</v>
+        <v>71186400</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40">
-        <v>124.6800003051758</v>
+        <v>126.5299987792969</v>
       </c>
       <c r="B40">
-        <v>124.8499984741211</v>
+        <v>127.4400024414062</v>
       </c>
       <c r="C40">
-        <v>123.129997253418</v>
+        <v>126.0999984741211</v>
       </c>
       <c r="D40">
-        <v>123.5400009155273</v>
+        <v>127.3499984741211</v>
       </c>
       <c r="E40">
-        <v>123.3551864624023</v>
+        <v>127.1594772338867</v>
       </c>
       <c r="F40">
-        <v>76229200</v>
+        <v>53522400</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41">
-        <v>124.0699996948242</v>
+        <v>127.8199996948242</v>
       </c>
       <c r="B41">
-        <v>126.1600036621094</v>
+        <v>130.5399932861328</v>
       </c>
       <c r="C41">
-        <v>123.8499984741211</v>
+        <v>127.0699996948242</v>
       </c>
       <c r="D41">
-        <v>125.8899993896484</v>
+        <v>130.4799957275391</v>
       </c>
       <c r="E41">
-        <v>125.7016677856445</v>
+        <v>130.2847900390625</v>
       </c>
       <c r="F41">
-        <v>75169300</v>
+        <v>96906500</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42">
-        <v>126.1699981689453</v>
+        <v>129.9400024414062</v>
       </c>
       <c r="B42">
-        <v>126.3199996948242</v>
+        <v>130.6000061035156</v>
       </c>
       <c r="C42">
-        <v>124.8300018310547</v>
+        <v>129.3899993896484</v>
       </c>
       <c r="D42">
-        <v>125.9000015258789</v>
+        <v>129.6399993896484</v>
       </c>
       <c r="E42">
-        <v>125.7116546630859</v>
+        <v>129.4460601806641</v>
       </c>
       <c r="F42">
-        <v>71057600</v>
+        <v>62746300</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
-        <v>126.5999984741211</v>
+        <v>130.3699951171875</v>
       </c>
       <c r="B43">
+        <v>130.8899993896484</v>
+      </c>
+      <c r="C43">
         <v>128.4600067138672</v>
       </c>
-      <c r="C43">
-        <v>126.2099990844727</v>
-      </c>
       <c r="D43">
-        <v>126.7399978637695</v>
+        <v>130.1499938964844</v>
       </c>
       <c r="E43">
-        <v>126.5503921508789</v>
+        <v>129.9552917480469</v>
       </c>
       <c r="F43">
-        <v>74403800</v>
+        <v>91815000</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
-        <v>127.2099990844727</v>
+        <v>129.8000030517578</v>
       </c>
       <c r="B44">
-        <v>127.75</v>
+        <v>132.5500030517578</v>
       </c>
       <c r="C44">
-        <v>126.5199966430664</v>
+        <v>129.6499938964844</v>
       </c>
       <c r="D44">
-        <v>127.129997253418</v>
+        <v>131.7899932861328</v>
       </c>
       <c r="E44">
-        <v>126.939811706543</v>
+        <v>131.5928344726562</v>
       </c>
       <c r="F44">
-        <v>56877900</v>
+        <v>96721700</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45">
-        <v>127.0199966430664</v>
+        <v>130.7100067138672</v>
       </c>
       <c r="B45">
-        <v>128.1900024414062</v>
+        <v>131.5099945068359</v>
       </c>
       <c r="C45">
-        <v>125.9400024414062</v>
+        <v>130.2400054931641</v>
       </c>
       <c r="D45">
-        <v>126.1100006103516</v>
+        <v>130.4600067138672</v>
       </c>
       <c r="E45">
-        <v>125.9213409423828</v>
+        <v>130.2648315429688</v>
       </c>
       <c r="F45">
-        <v>71186400</v>
+        <v>108953300</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
-        <v>126.5299987792969</v>
+        <v>130.3000030517578</v>
       </c>
       <c r="B46">
-        <v>127.4400024414062</v>
+        <v>132.4100036621094</v>
       </c>
       <c r="C46">
-        <v>126.0999984741211</v>
+        <v>129.2100067138672</v>
       </c>
       <c r="D46">
-        <v>127.3499984741211</v>
+        <v>132.3000030517578</v>
       </c>
       <c r="E46">
-        <v>127.1594772338867</v>
+        <v>132.1020812988281</v>
       </c>
       <c r="F46">
-        <v>53522400</v>
+        <v>79663300</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>127.8199996948242</v>
+        <v>132.1300048828125</v>
       </c>
       <c r="B47">
-        <v>130.5399932861328</v>
+        <v>134.0800018310547</v>
       </c>
       <c r="C47">
-        <v>127.0699996948242</v>
+        <v>131.6199951171875</v>
       </c>
       <c r="D47">
-        <v>130.4799957275391</v>
+        <v>133.9799957275391</v>
       </c>
       <c r="E47">
-        <v>130.2847900390625</v>
+        <v>133.7795562744141</v>
       </c>
       <c r="F47">
-        <v>96906500</v>
+        <v>74783600</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>129.9400024414062</v>
+        <v>133.7700042724609</v>
       </c>
       <c r="B48">
-        <v>130.6000061035156</v>
+        <v>134.3200073242188</v>
       </c>
       <c r="C48">
-        <v>129.3899993896484</v>
+        <v>133.2299957275391</v>
       </c>
       <c r="D48">
-        <v>129.6399993896484</v>
+        <v>133.6999969482422</v>
       </c>
       <c r="E48">
-        <v>129.4460601806641</v>
+        <v>133.4999847412109</v>
       </c>
       <c r="F48">
-        <v>62746300</v>
+        <v>60214200</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49">
-        <v>130.3699951171875</v>
+        <v>134.4499969482422</v>
       </c>
       <c r="B49">
-        <v>130.8899993896484</v>
+        <v>134.6399993896484</v>
       </c>
       <c r="C49">
-        <v>128.4600067138672</v>
+        <v>132.9299926757812</v>
       </c>
       <c r="D49">
-        <v>130.1499938964844</v>
+        <v>133.4100036621094</v>
       </c>
       <c r="E49">
-        <v>129.9552917480469</v>
+        <v>133.2104187011719</v>
       </c>
       <c r="F49">
-        <v>91815000</v>
+        <v>68711000</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50">
-        <v>129.8000030517578</v>
+        <v>133.4600067138672</v>
       </c>
       <c r="B50">
-        <v>132.5500030517578</v>
+        <v>133.8899993896484</v>
       </c>
       <c r="C50">
-        <v>129.6499938964844</v>
+        <v>132.8099975585938</v>
       </c>
       <c r="D50">
-        <v>131.7899932861328</v>
+        <v>133.1100006103516</v>
       </c>
       <c r="E50">
-        <v>131.5928344726562</v>
+        <v>132.9108734130859</v>
       </c>
       <c r="F50">
-        <v>96721700</v>
+        <v>70783700</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51">
-        <v>130.7100067138672</v>
+        <v>133.4100036621094</v>
       </c>
       <c r="B51">
-        <v>131.5099945068359</v>
+        <v>135.25</v>
       </c>
       <c r="C51">
-        <v>130.2400054931641</v>
+        <v>133.3500061035156</v>
       </c>
       <c r="D51">
-        <v>130.4600067138672</v>
+        <v>134.7799987792969</v>
       </c>
       <c r="E51">
-        <v>130.2648315429688</v>
+        <v>134.578369140625</v>
       </c>
       <c r="F51">
-        <v>108953300</v>
+        <v>62111300</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52">
-        <v>130.3000030517578</v>
+        <v>134.8000030517578</v>
       </c>
       <c r="B52">
-        <v>132.4100036621094</v>
+        <v>136.4900054931641</v>
       </c>
       <c r="C52">
-        <v>129.2100067138672</v>
+        <v>134.3500061035156</v>
       </c>
       <c r="D52">
-        <v>132.3000030517578</v>
+        <v>136.3300018310547</v>
       </c>
       <c r="E52">
-        <v>132.1020812988281</v>
+        <v>136.1260528564453</v>
       </c>
       <c r="F52">
-        <v>79663300</v>
+        <v>64556100</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53">
-        <v>132.1300048828125</v>
+        <v>136.1699981689453</v>
       </c>
       <c r="B53">
-        <v>134.0800018310547</v>
+        <v>137.4100036621094</v>
       </c>
       <c r="C53">
-        <v>131.6199951171875</v>
+        <v>135.8699951171875</v>
       </c>
       <c r="D53">
-        <v>133.9799957275391</v>
+        <v>136.9600067138672</v>
       </c>
       <c r="E53">
-        <v>133.7795562744141</v>
+        <v>136.7551116943359</v>
       </c>
       <c r="F53">
-        <v>74783600</v>
+        <v>63261400</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54">
-        <v>133.7700042724609</v>
+        <v>136.6000061035156</v>
       </c>
       <c r="B54">
-        <v>134.3200073242188</v>
+        <v>137.3300018310547</v>
       </c>
       <c r="C54">
-        <v>133.2299957275391</v>
+        <v>135.7599945068359</v>
       </c>
       <c r="D54">
-        <v>133.6999969482422</v>
+        <v>137.2700042724609</v>
       </c>
       <c r="E54">
-        <v>133.4999847412109</v>
+        <v>137.0646514892578</v>
       </c>
       <c r="F54">
-        <v>60214200</v>
+        <v>52485800</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55">
-        <v>134.4499969482422</v>
+        <v>137.8999938964844</v>
       </c>
       <c r="B55">
-        <v>134.6399993896484</v>
+        <v>140</v>
       </c>
       <c r="C55">
-        <v>132.9299926757812</v>
+        <v>137.75</v>
       </c>
       <c r="D55">
-        <v>133.4100036621094</v>
+        <v>139.9600067138672</v>
       </c>
       <c r="E55">
-        <v>133.2104187011719</v>
+        <v>139.7506256103516</v>
       </c>
       <c r="F55">
-        <v>68711000</v>
+        <v>78852600</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56">
-        <v>133.4600067138672</v>
+        <v>140.0700073242188</v>
       </c>
       <c r="B56">
-        <v>133.8899993896484</v>
+        <v>143.1499938964844</v>
       </c>
       <c r="C56">
-        <v>132.8099975585938</v>
+        <v>140.0700073242188</v>
       </c>
       <c r="D56">
-        <v>133.1100006103516</v>
+        <v>142.0200042724609</v>
       </c>
       <c r="E56">
-        <v>132.9108734130859</v>
+        <v>141.8075408935547</v>
       </c>
       <c r="F56">
-        <v>70783700</v>
+        <v>108181800</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57">
-        <v>133.4100036621094</v>
+        <v>143.5399932861328</v>
       </c>
       <c r="B57">
-        <v>135.25</v>
+        <v>144.8899993896484</v>
       </c>
       <c r="C57">
-        <v>133.3500061035156</v>
+        <v>142.6600036621094</v>
       </c>
       <c r="D57">
-        <v>134.7799987792969</v>
+        <v>144.5700073242188</v>
       </c>
       <c r="E57">
-        <v>134.578369140625</v>
+        <v>144.3537292480469</v>
       </c>
       <c r="F57">
-        <v>62111300</v>
+        <v>104911600</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58">
-        <v>134.8000030517578</v>
+        <v>141.5800018310547</v>
       </c>
       <c r="B58">
-        <v>136.4900054931641</v>
+        <v>144.0599975585938</v>
       </c>
       <c r="C58">
-        <v>134.3500061035156</v>
+        <v>140.6699981689453</v>
       </c>
       <c r="D58">
-        <v>136.3300018310547</v>
+        <v>143.2400054931641</v>
       </c>
       <c r="E58">
-        <v>136.1260528564453</v>
+        <v>143.0257110595703</v>
       </c>
       <c r="F58">
-        <v>64556100</v>
+        <v>105575500</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59">
-        <v>136.1699981689453</v>
+        <v>142.75</v>
       </c>
       <c r="B59">
-        <v>137.4100036621094</v>
+        <v>145.6499938964844</v>
       </c>
       <c r="C59">
-        <v>135.8699951171875</v>
+        <v>142.6499938964844</v>
       </c>
       <c r="D59">
-        <v>136.9600067138672</v>
+        <v>145.1100006103516</v>
       </c>
       <c r="E59">
-        <v>136.7551116943359</v>
+        <v>144.8929138183594</v>
       </c>
       <c r="F59">
-        <v>63261400</v>
+        <v>99890800</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60">
-        <v>136.6000061035156</v>
+        <v>146.2100067138672</v>
       </c>
       <c r="B60">
-        <v>137.3300018310547</v>
+        <v>146.3200073242188</v>
       </c>
       <c r="C60">
-        <v>135.7599945068359</v>
+        <v>144</v>
       </c>
       <c r="D60">
-        <v>137.2700042724609</v>
+        <v>144.5</v>
       </c>
       <c r="E60">
-        <v>137.0646514892578</v>
+        <v>144.2838287353516</v>
       </c>
       <c r="F60">
-        <v>52485800</v>
+        <v>76299700</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61">
-        <v>137.8999938964844</v>
+        <v>144.0299987792969</v>
       </c>
       <c r="B61">
-        <v>140</v>
+        <v>147.4600067138672</v>
       </c>
       <c r="C61">
-        <v>137.75</v>
+        <v>143.6300048828125</v>
       </c>
       <c r="D61">
-        <v>139.9600067138672</v>
+        <v>145.6399993896484</v>
       </c>
       <c r="E61">
-        <v>139.7506256103516</v>
+        <v>145.422119140625</v>
       </c>
       <c r="F61">
-        <v>78852600</v>
+        <v>100827100</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62">
-        <v>140.0700073242188</v>
+        <v>148.1000061035156</v>
       </c>
       <c r="B62">
-        <v>143.1499938964844</v>
+        <v>149.5700073242188</v>
       </c>
       <c r="C62">
-        <v>140.0700073242188</v>
+        <v>147.6799926757812</v>
       </c>
       <c r="D62">
-        <v>142.0200042724609</v>
+        <v>149.1499938964844</v>
       </c>
       <c r="E62">
-        <v>141.8075408935547</v>
+        <v>148.9268646240234</v>
       </c>
       <c r="F62">
-        <v>108181800</v>
+        <v>127050800</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63">
-        <v>143.5399932861328</v>
+        <v>149.2400054931641</v>
       </c>
       <c r="B63">
-        <v>144.8899993896484</v>
+        <v>150</v>
       </c>
       <c r="C63">
-        <v>142.6600036621094</v>
+        <v>147.0899963378906</v>
       </c>
       <c r="D63">
-        <v>144.5700073242188</v>
+        <v>148.4799957275391</v>
       </c>
       <c r="E63">
-        <v>144.3537292480469</v>
+        <v>148.2578735351562</v>
       </c>
       <c r="F63">
-        <v>104911600</v>
+        <v>106820300</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64">
-        <v>141.5800018310547</v>
+        <v>148.4600067138672</v>
       </c>
       <c r="B64">
-        <v>144.0599975585938</v>
+        <v>149.7599945068359</v>
       </c>
       <c r="C64">
-        <v>140.6699981689453</v>
+        <v>145.8800048828125</v>
       </c>
       <c r="D64">
-        <v>143.2400054931641</v>
+        <v>146.3899993896484</v>
       </c>
       <c r="E64">
-        <v>143.0257110595703</v>
+        <v>146.1709899902344</v>
       </c>
       <c r="F64">
-        <v>105575500</v>
+        <v>93251400</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65">
-        <v>142.75</v>
+        <v>143.75</v>
       </c>
       <c r="B65">
-        <v>145.6499938964844</v>
+        <v>144.0700073242188</v>
       </c>
       <c r="C65">
-        <v>142.6499938964844</v>
+        <v>141.6699981689453</v>
       </c>
       <c r="D65">
-        <v>145.1100006103516</v>
+        <v>142.4499969482422</v>
       </c>
       <c r="E65">
-        <v>144.8929138183594</v>
+        <v>142.2368927001953</v>
       </c>
       <c r="F65">
-        <v>99890800</v>
+        <v>121434600</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66">
-        <v>146.2100067138672</v>
+        <v>143.4600067138672</v>
       </c>
       <c r="B66">
-        <v>146.3200073242188</v>
+        <v>147.1000061035156</v>
       </c>
       <c r="C66">
-        <v>144</v>
+        <v>142.9600067138672</v>
       </c>
       <c r="D66">
-        <v>144.5</v>
+        <v>146.1499938964844</v>
       </c>
       <c r="E66">
-        <v>144.2838287353516</v>
+        <v>145.9313507080078</v>
       </c>
       <c r="F66">
-        <v>76299700</v>
+        <v>96350000</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67">
-        <v>144.0299987792969</v>
+        <v>145.5299987792969</v>
       </c>
       <c r="B67">
-        <v>147.4600067138672</v>
+        <v>146.1300048828125</v>
       </c>
       <c r="C67">
-        <v>143.6300048828125</v>
+        <v>144.6300048828125</v>
       </c>
       <c r="D67">
-        <v>145.6399993896484</v>
+        <v>145.3999938964844</v>
       </c>
       <c r="E67">
-        <v>145.422119140625</v>
+        <v>145.1824798583984</v>
       </c>
       <c r="F67">
-        <v>100827100</v>
+        <v>74993500</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68">
-        <v>148.1000061035156</v>
+        <v>145.9400024414062</v>
       </c>
       <c r="B68">
-        <v>149.5700073242188</v>
+        <v>148.1999969482422</v>
       </c>
       <c r="C68">
-        <v>147.6799926757812</v>
+        <v>145.8099975585938</v>
       </c>
       <c r="D68">
-        <v>149.1499938964844</v>
+        <v>146.8000030517578</v>
       </c>
       <c r="E68">
-        <v>148.9268646240234</v>
+        <v>146.5803833007812</v>
       </c>
       <c r="F68">
-        <v>127050800</v>
+        <v>77338200</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69">
-        <v>149.2400054931641</v>
+        <v>147.5500030517578</v>
       </c>
       <c r="B69">
-        <v>150</v>
+        <v>148.7200012207031</v>
       </c>
       <c r="C69">
-        <v>147.0899963378906</v>
+        <v>146.9199981689453</v>
       </c>
       <c r="D69">
-        <v>148.4799957275391</v>
+        <v>148.5599975585938</v>
       </c>
       <c r="E69">
-        <v>148.2578735351562</v>
+        <v>148.3377532958984</v>
       </c>
       <c r="F69">
-        <v>106820300</v>
+        <v>71447400</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70">
-        <v>148.4600067138672</v>
+        <v>148.2700042724609</v>
       </c>
       <c r="B70">
-        <v>149.7599945068359</v>
+        <v>149.8300018310547</v>
       </c>
       <c r="C70">
-        <v>145.8800048828125</v>
+        <v>147.6999969482422</v>
       </c>
       <c r="D70">
-        <v>146.3899993896484</v>
+        <v>148.9900054931641</v>
       </c>
       <c r="E70">
-        <v>146.1709899902344</v>
+        <v>148.7671203613281</v>
       </c>
       <c r="F70">
-        <v>93251400</v>
+        <v>72434100</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71">
-        <v>143.75</v>
+        <v>149.1199951171875</v>
       </c>
       <c r="B71">
-        <v>144.0700073242188</v>
+        <v>149.2100067138672</v>
       </c>
       <c r="C71">
-        <v>141.6699981689453</v>
+        <v>145.5500030517578</v>
       </c>
       <c r="D71">
-        <v>142.4499969482422</v>
+        <v>146.7700042724609</v>
       </c>
       <c r="E71">
-        <v>142.2368927001953</v>
+        <v>146.5504302978516</v>
       </c>
       <c r="F71">
-        <v>121434600</v>
+        <v>104818600</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72">
-        <v>143.4600067138672</v>
+        <v>144.8099975585938</v>
       </c>
       <c r="B72">
-        <v>147.1000061035156</v>
+        <v>146.9700012207031</v>
       </c>
       <c r="C72">
-        <v>142.9600067138672</v>
+        <v>142.5399932861328</v>
       </c>
       <c r="D72">
-        <v>146.1499938964844</v>
+        <v>144.9799957275391</v>
       </c>
       <c r="E72">
-        <v>145.9313507080078</v>
+        <v>144.7631072998047</v>
       </c>
       <c r="F72">
-        <v>96350000</v>
+        <v>118931200</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73">
-        <v>145.5299987792969</v>
+        <v>144.6900024414062</v>
       </c>
       <c r="B73">
-        <v>146.1300048828125</v>
+        <v>146.5500030517578</v>
       </c>
       <c r="C73">
-        <v>144.6300048828125</v>
+        <v>144.5800018310547</v>
       </c>
       <c r="D73">
-        <v>145.3999938964844</v>
+        <v>145.6399993896484</v>
       </c>
       <c r="E73">
-        <v>145.1824798583984</v>
+        <v>145.422119140625</v>
       </c>
       <c r="F73">
-        <v>74993500</v>
+        <v>56699500</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74">
-        <v>145.9400024414062</v>
+        <v>144.3800048828125</v>
       </c>
       <c r="B74">
-        <v>148.1999969482422</v>
+        <v>146.3300018310547</v>
       </c>
       <c r="C74">
-        <v>145.8099975585938</v>
+        <v>144.1100006103516</v>
       </c>
       <c r="D74">
-        <v>146.8000030517578</v>
+        <v>145.8600006103516</v>
       </c>
       <c r="E74">
-        <v>146.5803833007812</v>
+        <v>145.6417846679688</v>
       </c>
       <c r="F74">
-        <v>77338200</v>
+        <v>70382000</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75">
-        <v>147.5500030517578</v>
+        <v>146.3600006103516</v>
       </c>
       <c r="B75">
-        <v>148.7200012207031</v>
+        <v>146.9499969482422</v>
       </c>
       <c r="C75">
-        <v>146.9199981689453</v>
+        <v>145.25</v>
       </c>
       <c r="D75">
-        <v>148.5599975585938</v>
+        <v>145.5200042724609</v>
       </c>
       <c r="E75">
-        <v>148.3377532958984</v>
+        <v>145.3023071289062</v>
       </c>
       <c r="F75">
-        <v>71447400</v>
+        <v>62880000</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76">
-        <v>148.2700042724609</v>
+        <v>145.8099975585938</v>
       </c>
       <c r="B76">
-        <v>149.8300018310547</v>
+        <v>148.0399932861328</v>
       </c>
       <c r="C76">
-        <v>147.6999969482422</v>
+        <v>145.1799926757812</v>
       </c>
       <c r="D76">
-        <v>148.9900054931641</v>
+        <v>147.3600006103516</v>
       </c>
       <c r="E76">
-        <v>148.7671203613281</v>
+        <v>147.1395416259766</v>
       </c>
       <c r="F76">
-        <v>72434100</v>
+        <v>64786600</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77">
-        <v>149.1199951171875</v>
+        <v>147.2700042724609</v>
       </c>
       <c r="B77">
-        <v>149.2100067138672</v>
+        <v>147.7899932861328</v>
       </c>
       <c r="C77">
-        <v>145.5500030517578</v>
+        <v>146.2799987792969</v>
       </c>
       <c r="D77">
-        <v>146.7700042724609</v>
+        <v>146.9499969482422</v>
       </c>
       <c r="E77">
-        <v>146.5504302978516</v>
+        <v>146.7301635742188</v>
       </c>
       <c r="F77">
-        <v>104818600</v>
+        <v>56368300</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78">
-        <v>144.8099975585938</v>
+        <v>146.9799957275391</v>
       </c>
       <c r="B78">
-        <v>146.9700012207031</v>
+        <v>147.8399963378906</v>
       </c>
       <c r="C78">
-        <v>142.5399932861328</v>
+        <v>146.1699981689453</v>
       </c>
       <c r="D78">
-        <v>144.9799957275391</v>
+        <v>147.0599975585938</v>
       </c>
       <c r="E78">
-        <v>144.7631072998047</v>
+        <v>146.8399963378906</v>
       </c>
       <c r="F78">
-        <v>118931200</v>
+        <v>46397700</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79">
-        <v>144.6900024414062</v>
+        <v>146.3500061035156</v>
       </c>
       <c r="B79">
-        <v>146.5500030517578</v>
+        <v>147.1100006103516</v>
       </c>
       <c r="C79">
-        <v>144.5800018310547</v>
+        <v>145.6300048828125</v>
       </c>
       <c r="D79">
-        <v>145.6399993896484</v>
+        <v>146.1399993896484</v>
       </c>
       <c r="E79">
-        <v>145.422119140625</v>
+        <v>146.1399993896484</v>
       </c>
       <c r="F79">
-        <v>56699500</v>
+        <v>54067400</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80">
-        <v>144.3800048828125</v>
+        <v>146.1999969482422</v>
       </c>
       <c r="B80">
-        <v>146.3300018310547</v>
+        <v>146.6999969482422</v>
       </c>
       <c r="C80">
-        <v>144.1100006103516</v>
+        <v>145.5200042724609</v>
       </c>
       <c r="D80">
-        <v>145.8600006103516</v>
+        <v>146.0899963378906</v>
       </c>
       <c r="E80">
-        <v>145.6417846679688</v>
+        <v>146.0899963378906</v>
       </c>
       <c r="F80">
-        <v>70382000</v>
+        <v>48908700</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81">
-        <v>146.3600006103516</v>
+        <v>146.4400024414062</v>
       </c>
       <c r="B81">
-        <v>146.9499969482422</v>
+        <v>147.7100067138672</v>
       </c>
       <c r="C81">
-        <v>145.25</v>
+        <v>145.3000030517578</v>
       </c>
       <c r="D81">
-        <v>145.5200042724609</v>
+        <v>145.6000061035156</v>
       </c>
       <c r="E81">
-        <v>145.3023071289062</v>
+        <v>145.6000061035156</v>
       </c>
       <c r="F81">
-        <v>62880000</v>
+        <v>69023100</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82">
-        <v>145.8099975585938</v>
+        <v>146.0500030517578</v>
       </c>
       <c r="B82">
-        <v>148.0399932861328</v>
+        <v>146.7200012207031</v>
       </c>
       <c r="C82">
-        <v>145.1799926757812</v>
+        <v>145.5299987792969</v>
       </c>
       <c r="D82">
-        <v>147.3600006103516</v>
+        <v>145.8600006103516</v>
       </c>
       <c r="E82">
-        <v>147.1395416259766</v>
+        <v>145.8600006103516</v>
       </c>
       <c r="F82">
-        <v>64786600</v>
+        <v>48493500</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83">
-        <v>147.2700042724609</v>
+        <v>146.1900024414062</v>
       </c>
       <c r="B83">
-        <v>147.7899932861328</v>
+        <v>149.0500030517578</v>
       </c>
       <c r="C83">
-        <v>146.2799987792969</v>
+        <v>145.8399963378906</v>
       </c>
       <c r="D83">
-        <v>146.9499969482422</v>
+        <v>148.8899993896484</v>
       </c>
       <c r="E83">
-        <v>146.7301635742188</v>
+        <v>148.8899993896484</v>
       </c>
       <c r="F83">
-        <v>56368300</v>
+        <v>72282600</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84">
-        <v>146.9799957275391</v>
+        <v>148.9700012207031</v>
       </c>
       <c r="B84">
-        <v>147.8399963378906</v>
+        <v>149.4400024414062</v>
       </c>
       <c r="C84">
-        <v>146.1699981689453</v>
+        <v>148.2700042724609</v>
       </c>
       <c r="D84">
-        <v>147.0599975585938</v>
+        <v>149.1000061035156</v>
       </c>
       <c r="E84">
-        <v>146.8399963378906</v>
+        <v>149.1000061035156</v>
       </c>
       <c r="F84">
-        <v>46397700</v>
+        <v>59318800</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85">
-        <v>146.3500061035156</v>
+        <v>148.5399932861328</v>
       </c>
       <c r="B85">
-        <v>147.1100006103516</v>
+        <v>151.1900024414062</v>
       </c>
       <c r="C85">
-        <v>145.6300048828125</v>
+        <v>146.4700012207031</v>
       </c>
       <c r="D85">
-        <v>146.1399993896484</v>
+        <v>151.1199951171875</v>
       </c>
       <c r="E85">
-        <v>146.1399993896484</v>
+        <v>151.1199951171875</v>
       </c>
       <c r="F85">
-        <v>54067400</v>
+        <v>103296000</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86">
-        <v>146.1999969482422</v>
+        <v>150.2299957275391</v>
       </c>
       <c r="B86">
-        <v>146.6999969482422</v>
+        <v>151.6799926757812</v>
       </c>
       <c r="C86">
-        <v>145.5200042724609</v>
+        <v>149.0899963378906</v>
       </c>
       <c r="D86">
-        <v>146.0899963378906</v>
+        <v>150.1900024414062</v>
       </c>
       <c r="E86">
-        <v>146.0899963378906</v>
+        <v>150.1900024414062</v>
       </c>
       <c r="F86">
-        <v>48908700</v>
+        <v>92229700</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87">
-        <v>146.4400024414062</v>
+        <v>149.8000030517578</v>
       </c>
       <c r="B87">
-        <v>147.7100067138672</v>
+        <v>150.7200012207031</v>
       </c>
       <c r="C87">
-        <v>145.3000030517578</v>
+        <v>146.1499938964844</v>
       </c>
       <c r="D87">
-        <v>145.6000061035156</v>
+        <v>146.3600006103516</v>
       </c>
       <c r="E87">
-        <v>145.6000061035156</v>
+        <v>146.3600006103516</v>
       </c>
       <c r="F87">
-        <v>69023100</v>
+        <v>86326000</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88">
-        <v>146.0500030517578</v>
+        <v>145.0299987792969</v>
       </c>
       <c r="B88">
-        <v>146.7200012207031</v>
+        <v>148</v>
       </c>
       <c r="C88">
-        <v>145.5299987792969</v>
+        <v>144.5</v>
       </c>
       <c r="D88">
-        <v>145.8600006103516</v>
+        <v>146.6999969482422</v>
       </c>
       <c r="E88">
-        <v>145.8600006103516</v>
+        <v>146.6999969482422</v>
       </c>
       <c r="F88">
-        <v>48493500</v>
+        <v>86960300</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89">
-        <v>146.1900024414062</v>
+        <v>147.4400024414062</v>
       </c>
       <c r="B89">
-        <v>149.0500030517578</v>
+        <v>148.5</v>
       </c>
       <c r="C89">
-        <v>145.8399963378906</v>
+        <v>146.7799987792969</v>
       </c>
       <c r="D89">
-        <v>148.8899993896484</v>
+        <v>148.1900024414062</v>
       </c>
       <c r="E89">
-        <v>148.8899993896484</v>
+        <v>148.1900024414062</v>
       </c>
       <c r="F89">
-        <v>72282600</v>
+        <v>59947400</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90">
-        <v>148.9700012207031</v>
+        <v>148.3099975585938</v>
       </c>
       <c r="B90">
-        <v>149.4400024414062</v>
+        <v>150.1900024414062</v>
       </c>
       <c r="C90">
-        <v>148.2700042724609</v>
+        <v>147.8899993896484</v>
       </c>
       <c r="D90">
-        <v>149.1000061035156</v>
+        <v>149.7100067138672</v>
       </c>
       <c r="E90">
-        <v>149.1000061035156</v>
+        <v>149.7100067138672</v>
       </c>
       <c r="F90">
-        <v>59318800</v>
+        <v>60131800</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91">
-        <v>148.5399932861328</v>
+        <v>149.4499969482422</v>
       </c>
       <c r="B91">
-        <v>151.1900024414062</v>
+        <v>150.8600006103516</v>
       </c>
       <c r="C91">
-        <v>146.4700012207031</v>
+        <v>149.1499938964844</v>
       </c>
       <c r="D91">
-        <v>151.1199951171875</v>
+        <v>149.6199951171875</v>
       </c>
       <c r="E91">
-        <v>151.1199951171875</v>
+        <v>149.6199951171875</v>
       </c>
       <c r="F91">
-        <v>103296000</v>
+        <v>48606400</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92">
-        <v>150.2299957275391</v>
+        <v>149.8099975585938</v>
       </c>
       <c r="B92">
-        <v>151.6799926757812</v>
+        <v>150.3200073242188</v>
       </c>
       <c r="C92">
-        <v>149.0899963378906</v>
+        <v>147.8000030517578</v>
       </c>
       <c r="D92">
-        <v>150.1900024414062</v>
+        <v>148.3600006103516</v>
       </c>
       <c r="E92">
-        <v>150.1900024414062</v>
+        <v>148.3600006103516</v>
       </c>
       <c r="F92">
-        <v>92229700</v>
+        <v>58991300</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93">
-        <v>149.8000030517578</v>
+        <v>148.3500061035156</v>
       </c>
       <c r="B93">
-        <v>150.7200012207031</v>
+        <v>149.1199951171875</v>
       </c>
       <c r="C93">
-        <v>146.1499938964844</v>
+        <v>147.5099945068359</v>
       </c>
       <c r="D93">
-        <v>146.3600006103516</v>
+        <v>147.5399932861328</v>
       </c>
       <c r="E93">
-        <v>146.3600006103516</v>
+        <v>147.5399932861328</v>
       </c>
       <c r="F93">
-        <v>86326000</v>
+        <v>48597200</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94">
-        <v>145.0299987792969</v>
+        <v>147.4799957275391</v>
       </c>
       <c r="B94">
-        <v>148</v>
+        <v>148.75</v>
       </c>
       <c r="C94">
-        <v>144.5</v>
+        <v>146.8300018310547</v>
       </c>
       <c r="D94">
-        <v>146.6999969482422</v>
+        <v>148.6000061035156</v>
       </c>
       <c r="E94">
-        <v>146.6999969482422</v>
+        <v>148.6000061035156</v>
       </c>
       <c r="F94">
-        <v>86960300</v>
+        <v>55721500</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95">
-        <v>147.4400024414062</v>
+        <v>149</v>
       </c>
       <c r="B95">
-        <v>148.5</v>
+        <v>153.4900054931641</v>
       </c>
       <c r="C95">
-        <v>146.7799987792969</v>
+        <v>148.6100006103516</v>
       </c>
       <c r="D95">
-        <v>148.1900024414062</v>
+        <v>153.1199951171875</v>
       </c>
       <c r="E95">
-        <v>148.1900024414062</v>
+        <v>153.1199951171875</v>
       </c>
       <c r="F95">
-        <v>59947400</v>
+        <v>90956700</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96">
-        <v>148.3099975585938</v>
+        <v>152.6600036621094</v>
       </c>
       <c r="B96">
-        <v>150.1900024414062</v>
+        <v>152.8000030517578</v>
       </c>
       <c r="C96">
-        <v>147.8899993896484</v>
+        <v>151.2899932861328</v>
       </c>
       <c r="D96">
-        <v>149.7100067138672</v>
+        <v>151.8300018310547</v>
       </c>
       <c r="E96">
-        <v>149.7100067138672</v>
+        <v>151.8300018310547</v>
       </c>
       <c r="F96">
-        <v>60131800</v>
+        <v>86453100</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97">
-        <v>149.4499969482422</v>
+        <v>152.8300018310547</v>
       </c>
       <c r="B97">
-        <v>150.8600006103516</v>
+        <v>154.9799957275391</v>
       </c>
       <c r="C97">
-        <v>149.1499938964844</v>
+        <v>152.3399963378906</v>
       </c>
       <c r="D97">
-        <v>149.6199951171875</v>
+        <v>152.5099945068359</v>
       </c>
       <c r="E97">
-        <v>149.6199951171875</v>
+        <v>152.5099945068359</v>
       </c>
       <c r="F97">
-        <v>48606400</v>
+        <v>80313700</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98">
-        <v>149.8099975585938</v>
+        <v>153.8699951171875</v>
       </c>
       <c r="B98">
-        <v>150.3200073242188</v>
+        <v>154.7200012207031</v>
       </c>
       <c r="C98">
-        <v>147.8000030517578</v>
+        <v>152.3999938964844</v>
       </c>
       <c r="D98">
-        <v>148.3600006103516</v>
+        <v>153.6499938964844</v>
       </c>
       <c r="E98">
-        <v>148.3600006103516</v>
+        <v>153.6499938964844</v>
       </c>
       <c r="F98">
-        <v>58991300</v>
+        <v>71115500</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99">
-        <v>148.3500061035156</v>
+        <v>153.7599945068359</v>
       </c>
       <c r="B99">
-        <v>149.1199951171875</v>
+        <v>154.6300048828125</v>
       </c>
       <c r="C99">
-        <v>147.5099945068359</v>
+        <v>153.0899963378906</v>
       </c>
       <c r="D99">
-        <v>147.5399932861328</v>
+        <v>154.3000030517578</v>
       </c>
       <c r="E99">
-        <v>147.5399932861328</v>
+        <v>154.3000030517578</v>
       </c>
       <c r="F99">
-        <v>48597200</v>
+        <v>57808700</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100">
-        <v>147.4799957275391</v>
+        <v>154.9700012207031</v>
       </c>
       <c r="B100">
-        <v>148.75</v>
+        <v>157.2599945068359</v>
       </c>
       <c r="C100">
-        <v>146.8300018310547</v>
+        <v>154.3899993896484</v>
       </c>
       <c r="D100">
-        <v>148.6000061035156</v>
+        <v>156.6900024414062</v>
       </c>
       <c r="E100">
-        <v>148.6000061035156</v>
+        <v>156.6900024414062</v>
       </c>
       <c r="F100">
-        <v>55721500</v>
+        <v>82278300</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101">
-        <v>149</v>
+        <v>156.9799957275391</v>
       </c>
       <c r="B101">
-        <v>153.4900054931641</v>
+        <v>157.0399932861328</v>
       </c>
       <c r="C101">
-        <v>148.6100006103516</v>
+        <v>153.9799957275391</v>
       </c>
       <c r="D101">
-        <v>153.1199951171875</v>
+        <v>155.1100006103516</v>
       </c>
       <c r="E101">
-        <v>153.1199951171875</v>
+        <v>155.1100006103516</v>
       </c>
       <c r="F101">
-        <v>90956700</v>
+        <v>74420200</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102">
-        <v>152.6600036621094</v>
+        <v>155.4900054931641</v>
       </c>
       <c r="B102">
-        <v>152.8000030517578</v>
+        <v>156.1100006103516</v>
       </c>
       <c r="C102">
-        <v>151.2899932861328</v>
+        <v>153.9499969482422</v>
       </c>
       <c r="D102">
-        <v>151.8300018310547</v>
+        <v>154.0700073242188</v>
       </c>
       <c r="E102">
-        <v>151.8300018310547</v>
+        <v>154.0700073242188</v>
       </c>
       <c r="F102">
-        <v>86453100</v>
+        <v>57305700</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103">
-        <v>152.8300018310547</v>
+        <v>155</v>
       </c>
       <c r="B103">
-        <v>154.9799957275391</v>
+        <v>155.4799957275391</v>
       </c>
       <c r="C103">
-        <v>152.3399963378906</v>
+        <v>148.6999969482422</v>
       </c>
       <c r="D103">
-        <v>152.5099945068359</v>
+        <v>148.9700012207031</v>
       </c>
       <c r="E103">
-        <v>152.5099945068359</v>
+        <v>148.9700012207031</v>
       </c>
       <c r="F103">
-        <v>80313700</v>
+        <v>140646400</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104">
-        <v>153.8699951171875</v>
+        <v>150.6300048828125</v>
       </c>
       <c r="B104">
-        <v>154.7200012207031</v>
+        <v>151.4199981689453</v>
       </c>
       <c r="C104">
-        <v>152.3999938964844</v>
+        <v>148.75</v>
       </c>
       <c r="D104">
-        <v>153.6499938964844</v>
+        <v>149.5500030517578</v>
       </c>
       <c r="E104">
-        <v>153.6499938964844</v>
+        <v>149.5500030517578</v>
       </c>
       <c r="F104">
-        <v>71115500</v>
+        <v>102404300</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105">
-        <v>153.7599945068359</v>
+        <v>150.3500061035156</v>
       </c>
       <c r="B105">
-        <v>154.6300048828125</v>
+        <v>151.0700073242188</v>
       </c>
       <c r="C105">
-        <v>153.0899963378906</v>
+        <v>146.9100036621094</v>
       </c>
       <c r="D105">
-        <v>154.3000030517578</v>
+        <v>148.1199951171875</v>
       </c>
       <c r="E105">
-        <v>154.3000030517578</v>
+        <v>148.1199951171875</v>
       </c>
       <c r="F105">
-        <v>57808700</v>
+        <v>109296300</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106">
-        <v>154.9700012207031</v>
+        <v>148.5599975585938</v>
       </c>
       <c r="B106">
-        <v>157.2599945068359</v>
+        <v>149.4400024414062</v>
       </c>
       <c r="C106">
-        <v>154.3899993896484</v>
+        <v>146.3699951171875</v>
       </c>
       <c r="D106">
-        <v>156.6900024414062</v>
+        <v>149.0299987792969</v>
       </c>
       <c r="E106">
-        <v>156.6900024414062</v>
+        <v>149.0299987792969</v>
       </c>
       <c r="F106">
-        <v>82278300</v>
+        <v>83281300</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107">
-        <v>156.9799957275391</v>
+        <v>148.4400024414062</v>
       </c>
       <c r="B107">
-        <v>157.0399932861328</v>
+        <v>148.9700012207031</v>
       </c>
       <c r="C107">
-        <v>153.9799957275391</v>
+        <v>147.2200012207031</v>
       </c>
       <c r="D107">
-        <v>155.1100006103516</v>
+        <v>148.7899932861328</v>
       </c>
       <c r="E107">
-        <v>155.1100006103516</v>
+        <v>148.7899932861328</v>
       </c>
       <c r="F107">
-        <v>74420200</v>
+        <v>68034100</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108">
-        <v>155.4900054931641</v>
+        <v>148.8200073242188</v>
       </c>
       <c r="B108">
-        <v>156.1100006103516</v>
+        <v>148.8200073242188</v>
       </c>
       <c r="C108">
-        <v>153.9499969482422</v>
+        <v>145.7599945068359</v>
       </c>
       <c r="D108">
-        <v>154.0700073242188</v>
+        <v>146.0599975585938</v>
       </c>
       <c r="E108">
-        <v>154.0700073242188</v>
+        <v>146.0599975585938</v>
       </c>
       <c r="F108">
-        <v>57305700</v>
+        <v>129868800</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109">
-        <v>155</v>
+        <v>143.8000030517578</v>
       </c>
       <c r="B109">
-        <v>155.4799957275391</v>
+        <v>144.8399963378906</v>
       </c>
       <c r="C109">
-        <v>148.6999969482422</v>
+        <v>141.2700042724609</v>
       </c>
       <c r="D109">
-        <v>148.9700012207031</v>
+        <v>142.9400024414062</v>
       </c>
       <c r="E109">
-        <v>148.9700012207031</v>
+        <v>142.9400024414062</v>
       </c>
       <c r="F109">
-        <v>140646400</v>
+        <v>123478900</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110">
-        <v>150.6300048828125</v>
+        <v>143.9299926757812</v>
       </c>
       <c r="B110">
-        <v>151.4199981689453</v>
+        <v>144.6000061035156</v>
       </c>
       <c r="C110">
-        <v>148.75</v>
+        <v>142.7799987792969</v>
       </c>
       <c r="D110">
-        <v>149.5500030517578</v>
+        <v>143.4299926757812</v>
       </c>
       <c r="E110">
-        <v>149.5500030517578</v>
+        <v>143.4299926757812</v>
       </c>
       <c r="F110">
-        <v>102404300</v>
+        <v>75834000</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111">
-        <v>150.3500061035156</v>
+        <v>144.4499969482422</v>
       </c>
       <c r="B111">
-        <v>151.0700073242188</v>
+        <v>146.4299926757812</v>
       </c>
       <c r="C111">
-        <v>146.9100036621094</v>
+        <v>143.6999969482422</v>
       </c>
       <c r="D111">
-        <v>148.1199951171875</v>
+        <v>145.8500061035156</v>
       </c>
       <c r="E111">
-        <v>148.1199951171875</v>
+        <v>145.8500061035156</v>
       </c>
       <c r="F111">
-        <v>109296300</v>
+        <v>76404300</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112">
-        <v>148.5599975585938</v>
+        <v>146.6499938964844</v>
       </c>
       <c r="B112">
-        <v>149.4400024414062</v>
+        <v>147.0800018310547</v>
       </c>
       <c r="C112">
-        <v>146.3699951171875</v>
+        <v>145.6399993896484</v>
       </c>
       <c r="D112">
-        <v>149.0299987792969</v>
+        <v>146.8300018310547</v>
       </c>
       <c r="E112">
-        <v>149.0299987792969</v>
+        <v>146.8300018310547</v>
       </c>
       <c r="F112">
-        <v>83281300</v>
+        <v>64838200</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113">
-        <v>148.4400024414062</v>
+        <v>145.6600036621094</v>
       </c>
       <c r="B113">
-        <v>148.9700012207031</v>
+        <v>147.4700012207031</v>
       </c>
       <c r="C113">
-        <v>147.2200012207031</v>
+        <v>145.5599975585938</v>
       </c>
       <c r="D113">
-        <v>148.7899932861328</v>
+        <v>146.9199981689453</v>
       </c>
       <c r="E113">
-        <v>148.7899932861328</v>
+        <v>146.9199981689453</v>
       </c>
       <c r="F113">
-        <v>68034100</v>
+        <v>53477900</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114">
-        <v>148.8200073242188</v>
+        <v>145.4700012207031</v>
       </c>
       <c r="B114">
-        <v>148.8200073242188</v>
+        <v>145.9600067138672</v>
       </c>
       <c r="C114">
-        <v>145.7599945068359</v>
+        <v>143.8200073242188</v>
       </c>
       <c r="D114">
-        <v>146.0599975585938</v>
+        <v>145.3699951171875</v>
       </c>
       <c r="E114">
-        <v>146.0599975585938</v>
+        <v>145.3699951171875</v>
       </c>
       <c r="F114">
-        <v>129868800</v>
+        <v>74150700</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115">
-        <v>143.8000030517578</v>
+        <v>143.25</v>
       </c>
       <c r="B115">
-        <v>144.8399963378906</v>
+        <v>144.75</v>
       </c>
       <c r="C115">
-        <v>141.2700042724609</v>
+        <v>141.6900024414062</v>
       </c>
       <c r="D115">
-        <v>142.9400024414062</v>
+        <v>141.9100036621094</v>
       </c>
       <c r="E115">
-        <v>142.9400024414062</v>
+        <v>141.9100036621094</v>
       </c>
       <c r="F115">
-        <v>123478900</v>
+        <v>108972300</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116">
-        <v>143.9299926757812</v>
+        <v>142.4700012207031</v>
       </c>
       <c r="B116">
-        <v>144.6000061035156</v>
+        <v>144.4499969482422</v>
       </c>
       <c r="C116">
-        <v>142.7799987792969</v>
+        <v>142.0299987792969</v>
       </c>
       <c r="D116">
-        <v>143.4299926757812</v>
+        <v>142.8300018310547</v>
       </c>
       <c r="E116">
-        <v>143.4299926757812</v>
+        <v>142.8300018310547</v>
       </c>
       <c r="F116">
-        <v>75834000</v>
+        <v>74602000</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117">
-        <v>144.4499969482422</v>
+        <v>143.6600036621094</v>
       </c>
       <c r="B117">
-        <v>146.4299926757812</v>
+        <v>144.3800048828125</v>
       </c>
       <c r="C117">
-        <v>143.6999969482422</v>
+        <v>141.2799987792969</v>
       </c>
       <c r="D117">
-        <v>145.8500061035156</v>
+        <v>141.5</v>
       </c>
       <c r="E117">
-        <v>145.8500061035156</v>
+        <v>141.5</v>
       </c>
       <c r="F117">
-        <v>76404300</v>
+        <v>88934200</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118">
-        <v>146.6499938964844</v>
+        <v>141.8999938964844</v>
       </c>
       <c r="B118">
-        <v>147.0800018310547</v>
+        <v>142.9199981689453</v>
       </c>
       <c r="C118">
-        <v>145.6399993896484</v>
+        <v>139.1100006103516</v>
       </c>
       <c r="D118">
-        <v>146.8300018310547</v>
+        <v>142.6499938964844</v>
       </c>
       <c r="E118">
-        <v>146.8300018310547</v>
+        <v>142.6499938964844</v>
       </c>
       <c r="F118">
-        <v>64838200</v>
+        <v>94639600</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119">
-        <v>145.6600036621094</v>
+        <v>141.7599945068359</v>
       </c>
       <c r="B119">
-        <v>147.4700012207031</v>
+        <v>142.2100067138672</v>
       </c>
       <c r="C119">
-        <v>145.5599975585938</v>
+        <v>138.2700042724609</v>
       </c>
       <c r="D119">
-        <v>146.9199981689453</v>
+        <v>139.1399993896484</v>
       </c>
       <c r="E119">
-        <v>146.9199981689453</v>
+        <v>139.1399993896484</v>
       </c>
       <c r="F119">
-        <v>53477900</v>
+        <v>98322000</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120">
-        <v>145.4700012207031</v>
+        <v>139.4900054931641</v>
       </c>
       <c r="B120">
-        <v>145.9600067138672</v>
+        <v>142.2400054931641</v>
       </c>
       <c r="C120">
-        <v>143.8200073242188</v>
+        <v>139.3600006103516</v>
       </c>
       <c r="D120">
-        <v>145.3699951171875</v>
+        <v>141.1100006103516</v>
       </c>
       <c r="E120">
-        <v>145.3699951171875</v>
+        <v>141.1100006103516</v>
       </c>
       <c r="F120">
-        <v>74150700</v>
+        <v>80861100</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121">
-        <v>143.25</v>
+        <v>139.4700012207031</v>
       </c>
       <c r="B121">
-        <v>144.75</v>
+        <v>142.1499938964844</v>
       </c>
       <c r="C121">
-        <v>141.6900024414062</v>
+        <v>138.3699951171875</v>
       </c>
       <c r="D121">
-        <v>141.9100036621094</v>
+        <v>142</v>
       </c>
       <c r="E121">
-        <v>141.9100036621094</v>
+        <v>142</v>
       </c>
       <c r="F121">
-        <v>108972300</v>
+        <v>83221100</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122">
-        <v>142.4700012207031</v>
+        <v>143.0599975585938</v>
       </c>
       <c r="B122">
-        <v>144.4499969482422</v>
+        <v>144.2200012207031</v>
       </c>
       <c r="C122">
-        <v>142.0299987792969</v>
+        <v>142.7200012207031</v>
       </c>
       <c r="D122">
-        <v>142.8300018310547</v>
+        <v>143.2899932861328</v>
       </c>
       <c r="E122">
-        <v>142.8300018310547</v>
+        <v>143.2899932861328</v>
       </c>
       <c r="F122">
-        <v>74602000</v>
+        <v>61732700</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123">
-        <v>143.6600036621094</v>
+        <v>144.0299987792969</v>
       </c>
       <c r="B123">
-        <v>144.3800048828125</v>
+        <v>144.1799926757812</v>
       </c>
       <c r="C123">
-        <v>141.2799987792969</v>
+        <v>142.5599975585938</v>
       </c>
       <c r="D123">
-        <v>141.5</v>
+        <v>142.8999938964844</v>
       </c>
       <c r="E123">
-        <v>141.5</v>
+        <v>142.8999938964844</v>
       </c>
       <c r="F123">
-        <v>88934200</v>
+        <v>58718700</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="A124">
-        <v>141.8999938964844</v>
+        <v>142.2700042724609</v>
       </c>
       <c r="B124">
-        <v>142.9199981689453</v>
+        <v>144.8099975585938</v>
       </c>
       <c r="C124">
-        <v>139.1100006103516</v>
+        <v>141.8099975585938</v>
       </c>
       <c r="D124">
-        <v>142.6499938964844</v>
+        <v>142.8099975585938</v>
       </c>
       <c r="E124">
-        <v>142.6499938964844</v>
+        <v>142.8099975585938</v>
       </c>
       <c r="F124">
-        <v>94639600</v>
+        <v>64452200</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="A125">
-        <v>141.7599945068359</v>
+        <v>143.2299957275391</v>
       </c>
       <c r="B125">
-        <v>142.2100067138672</v>
+        <v>143.25</v>
       </c>
       <c r="C125">
-        <v>138.2700042724609</v>
+        <v>141.0399932861328</v>
       </c>
       <c r="D125">
-        <v>139.1399993896484</v>
+        <v>141.5099945068359</v>
       </c>
       <c r="E125">
-        <v>139.1399993896484</v>
+        <v>141.5099945068359</v>
       </c>
       <c r="F125">
-        <v>98322000</v>
+        <v>73035900</v>
       </c>
     </row>
     <row r="126" spans="1:6">
       <c r="A126">
-        <v>139.4900054931641</v>
+        <v>141.2400054931641</v>
       </c>
       <c r="B126">
-        <v>142.2400054931641</v>
+        <v>141.3999938964844</v>
       </c>
       <c r="C126">
-        <v>139.3600006103516</v>
+        <v>139.1999969482422</v>
       </c>
       <c r="D126">
-        <v>141.1100006103516</v>
+        <v>140.9100036621094</v>
       </c>
       <c r="E126">
-        <v>141.1100006103516</v>
+        <v>140.9100036621094</v>
       </c>
       <c r="F126">
-        <v>80861100</v>
+        <v>78762700</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127">
-        <v>139.4700012207031</v>
+        <v>142.1100006103516</v>
       </c>
       <c r="B127">
-        <v>142.1499938964844</v>
+        <v>143.8800048828125</v>
       </c>
       <c r="C127">
-        <v>138.3699951171875</v>
+        <v>141.5099945068359</v>
       </c>
       <c r="D127">
-        <v>142</v>
+        <v>143.7599945068359</v>
       </c>
       <c r="E127">
-        <v>142</v>
+        <v>143.7599945068359</v>
       </c>
       <c r="F127">
-        <v>83221100</v>
+        <v>69907100</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="A128">
-        <v>143.0599975585938</v>
+        <v>143.7700042724609</v>
       </c>
       <c r="B128">
-        <v>144.2200012207031</v>
+        <v>144.8999938964844</v>
       </c>
       <c r="C128">
-        <v>142.7200012207031</v>
+        <v>143.5099945068359</v>
       </c>
       <c r="D128">
-        <v>143.2899932861328</v>
+        <v>144.8399963378906</v>
       </c>
       <c r="E128">
-        <v>143.2899932861328</v>
+        <v>144.8399963378906</v>
       </c>
       <c r="F128">
-        <v>61732700</v>
+        <v>67885200</v>
       </c>
     </row>
     <row r="129" spans="1:6">
       <c r="A129">
-        <v>144.0299987792969</v>
+        <v>143.4450073242188</v>
       </c>
       <c r="B129">
-        <v>144.1799926757812</v>
+        <v>145.5198974609375</v>
       </c>
       <c r="C129">
-        <v>142.5599975585938</v>
+        <v>143.1600036621094</v>
       </c>
       <c r="D129">
-        <v>142.8999938964844</v>
+        <v>145.4649963378906</v>
       </c>
       <c r="E129">
-        <v>142.8999938964844</v>
+        <v>145.4649963378906</v>
       </c>
       <c r="F129">
-        <v>58718700</v>
+        <v>35743753</v>
       </c>
     </row>
   </sheetData>

</xml_diff>